<commit_message>
Choosen the phonemes and added data-gathering apps
</commit_message>
<xml_diff>
--- a/Silabel dan Data.xlsx
+++ b/Silabel dan Data.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabagita Ivan\Desktop\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CADD7960-B9AD-41A0-9AB3-D582B6962615}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2A07E1-CBB6-4D8A-BD83-A1AA5403C33C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{6A493B5F-695C-4F94-90D7-2C81C2950938}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="3" xr2:uid="{6A493B5F-695C-4F94-90D7-2C81C2950938}"/>
   </bookViews>
   <sheets>
     <sheet name="Silabel" sheetId="3" r:id="rId1"/>
     <sheet name="Data" sheetId="4" r:id="rId2"/>
+    <sheet name="&gt;=10 + Alphabet" sheetId="11" r:id="rId3"/>
+    <sheet name="Choosen Phoneme" sheetId="12" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="704">
   <si>
     <t>abad</t>
   </si>
@@ -2063,6 +2065,81 @@
   </si>
   <si>
     <t>lezat</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>oi</t>
+  </si>
+  <si>
+    <t>b bé</t>
+  </si>
+  <si>
+    <t>c cé</t>
+  </si>
+  <si>
+    <t>d dé</t>
+  </si>
+  <si>
+    <t>e é</t>
+  </si>
+  <si>
+    <t>g gé</t>
+  </si>
+  <si>
+    <t>h ha</t>
+  </si>
+  <si>
+    <t>j jé</t>
+  </si>
+  <si>
+    <t>k ka</t>
+  </si>
+  <si>
+    <t>f èf</t>
+  </si>
+  <si>
+    <t>l èl</t>
+  </si>
+  <si>
+    <t>m èm</t>
+  </si>
+  <si>
+    <t>n èn</t>
+  </si>
+  <si>
+    <t>p pé</t>
+  </si>
+  <si>
+    <t>q ki</t>
+  </si>
+  <si>
+    <t>r èr</t>
+  </si>
+  <si>
+    <t>s ès</t>
+  </si>
+  <si>
+    <t>t té</t>
+  </si>
+  <si>
+    <t>v vé</t>
+  </si>
+  <si>
+    <t>w wé</t>
+  </si>
+  <si>
+    <t>y yé</t>
+  </si>
+  <si>
+    <t>z zét</t>
+  </si>
+  <si>
+    <t>x èks</t>
+  </si>
+  <si>
+    <t>ei éi</t>
   </si>
 </sst>
 </file>
@@ -2431,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD56F896-83CB-4809-AA3D-0E83B405C63A}">
   <dimension ref="A1:B290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2442,154 +2519,154 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>373</v>
+        <v>422</v>
       </c>
       <c r="B1" s="2">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>554</v>
+        <v>393</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>643</v>
+        <v>621</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>384</v>
+        <v>399</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>528</v>
+        <v>421</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>632</v>
+        <v>486</v>
       </c>
       <c r="B6" s="2">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>448</v>
       </c>
       <c r="B7" s="2">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>391</v>
+        <v>454</v>
       </c>
       <c r="B8" s="2">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>431</v>
+        <v>498</v>
       </c>
       <c r="B9" s="2">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B11" s="2">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="B12" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>400</v>
+        <v>379</v>
       </c>
       <c r="B13" s="2">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>518</v>
+        <v>562</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B15" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B16" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>419</v>
+        <v>381</v>
       </c>
       <c r="B17" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>465</v>
+        <v>493</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>589</v>
+        <v>457</v>
       </c>
       <c r="B19" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2602,34 +2679,34 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>385</v>
+        <v>417</v>
       </c>
       <c r="B21" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>427</v>
+        <v>70</v>
       </c>
       <c r="B22" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>555</v>
+        <v>394</v>
       </c>
       <c r="B23" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>388</v>
+        <v>499</v>
       </c>
       <c r="B24" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2642,359 +2719,359 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>559</v>
+        <v>526</v>
       </c>
       <c r="B26" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>620</v>
+        <v>392</v>
       </c>
       <c r="B27" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="B28" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="B29" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>593</v>
+        <v>501</v>
       </c>
       <c r="B30" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>656</v>
+        <v>425</v>
       </c>
       <c r="B31" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>439</v>
+        <v>567</v>
       </c>
       <c r="B32" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>551</v>
+        <v>596</v>
       </c>
       <c r="B33" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>442</v>
+        <v>521</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>441</v>
+        <v>561</v>
       </c>
       <c r="B35" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="B36" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>417</v>
+        <v>527</v>
       </c>
       <c r="B37" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>375</v>
+        <v>563</v>
       </c>
       <c r="B38" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>494</v>
+        <v>449</v>
       </c>
       <c r="B39" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>594</v>
+        <v>552</v>
       </c>
       <c r="B40" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>397</v>
+        <v>459</v>
       </c>
       <c r="B41" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>476</v>
       </c>
       <c r="B42" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>519</v>
+        <v>481</v>
       </c>
       <c r="B43" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>564</v>
+        <v>444</v>
       </c>
       <c r="B44" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>657</v>
+        <v>495</v>
       </c>
       <c r="B45" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>447</v>
+        <v>541</v>
       </c>
       <c r="B46" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>482</v>
+        <v>389</v>
       </c>
       <c r="B47" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="B48" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>412</v>
       </c>
       <c r="B49" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>455</v>
+        <v>413</v>
       </c>
       <c r="B50" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>650</v>
+        <v>414</v>
       </c>
       <c r="B51" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>456</v>
+        <v>415</v>
       </c>
       <c r="B52" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>488</v>
+        <v>384</v>
       </c>
       <c r="B53" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>641</v>
+        <v>418</v>
       </c>
       <c r="B54" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>459</v>
+        <v>388</v>
       </c>
       <c r="B55" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>461</v>
+        <v>439</v>
       </c>
       <c r="B56" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>659</v>
+        <v>490</v>
       </c>
       <c r="B57" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>673</v>
+        <v>404</v>
       </c>
       <c r="B58" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>662</v>
+        <v>487</v>
       </c>
       <c r="B59" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="B60" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>463</v>
+        <v>511</v>
       </c>
       <c r="B61" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>663</v>
+        <v>514</v>
       </c>
       <c r="B62" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>470</v>
+        <v>496</v>
       </c>
       <c r="B63" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>469</v>
+        <v>380</v>
       </c>
       <c r="B64" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>667</v>
+        <v>582</v>
       </c>
       <c r="B65" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>668</v>
+        <v>408</v>
       </c>
       <c r="B66" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>473</v>
+        <v>556</v>
       </c>
       <c r="B67" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>520</v>
+        <v>433</v>
       </c>
       <c r="B68" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>640</v>
+        <v>529</v>
       </c>
       <c r="B69" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>490</v>
+        <v>537</v>
       </c>
       <c r="B70" s="2">
         <v>3</v>
@@ -3002,191 +3079,191 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="B71" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>655</v>
+        <v>390</v>
       </c>
       <c r="B72" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>376</v>
+        <v>592</v>
       </c>
       <c r="B73" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>660</v>
+        <v>617</v>
       </c>
       <c r="B74" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>476</v>
+        <v>387</v>
       </c>
       <c r="B75" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>477</v>
+        <v>432</v>
       </c>
       <c r="B76" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>479</v>
+        <v>424</v>
       </c>
       <c r="B77" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="B78" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>405</v>
+        <v>431</v>
       </c>
       <c r="B79" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>460</v>
+        <v>400</v>
       </c>
       <c r="B80" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>578</v>
+        <v>419</v>
       </c>
       <c r="B81" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>481</v>
+        <v>589</v>
       </c>
       <c r="B82" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>403</v>
+        <v>620</v>
       </c>
       <c r="B83" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>98</v>
+        <v>593</v>
       </c>
       <c r="B84" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>99</v>
+        <v>442</v>
       </c>
       <c r="B85" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>616</v>
+        <v>443</v>
       </c>
       <c r="B86" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>565</v>
+        <v>455</v>
       </c>
       <c r="B87" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>546</v>
+        <v>461</v>
       </c>
       <c r="B88" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>487</v>
+        <v>462</v>
       </c>
       <c r="B89" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>489</v>
+        <v>407</v>
       </c>
       <c r="B90" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>609</v>
+        <v>515</v>
       </c>
       <c r="B91" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>491</v>
+        <v>504</v>
       </c>
       <c r="B92" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>493</v>
+        <v>153</v>
       </c>
       <c r="B93" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>407</v>
+        <v>474</v>
       </c>
       <c r="B94" s="2">
         <v>2</v>
@@ -3194,103 +3271,103 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>452</v>
+        <v>524</v>
       </c>
       <c r="B95" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>377</v>
+        <v>610</v>
       </c>
       <c r="B96" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>497</v>
+        <v>548</v>
       </c>
       <c r="B97" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>420</v>
+        <v>440</v>
       </c>
       <c r="B98" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>625</v>
+        <v>502</v>
       </c>
       <c r="B99" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>492</v>
+        <v>468</v>
       </c>
       <c r="B100" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>661</v>
+        <v>450</v>
       </c>
       <c r="B101" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>511</v>
+        <v>483</v>
       </c>
       <c r="B102" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>512</v>
+        <v>602</v>
       </c>
       <c r="B103" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>579</v>
+        <v>453</v>
       </c>
       <c r="B104" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>514</v>
+        <v>598</v>
       </c>
       <c r="B105" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>644</v>
+        <v>464</v>
       </c>
       <c r="B106" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>515</v>
+        <v>597</v>
       </c>
       <c r="B107" s="2">
         <v>2</v>
@@ -3298,71 +3375,71 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>646</v>
+        <v>523</v>
       </c>
       <c r="B108" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>516</v>
+        <v>429</v>
       </c>
       <c r="B109" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>498</v>
+        <v>626</v>
       </c>
       <c r="B110" s="2">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>496</v>
+        <v>631</v>
       </c>
       <c r="B111" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>612</v>
+        <v>587</v>
       </c>
       <c r="B112" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>378</v>
+        <v>639</v>
       </c>
       <c r="B113" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>379</v>
+        <v>611</v>
       </c>
       <c r="B114" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>434</v>
+        <v>654</v>
       </c>
       <c r="B115" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>504</v>
+        <v>642</v>
       </c>
       <c r="B116" s="2">
         <v>2</v>
@@ -3370,23 +3447,23 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>544</v>
+        <v>445</v>
       </c>
       <c r="B117" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>423</v>
+        <v>542</v>
       </c>
       <c r="B118" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>153</v>
+        <v>508</v>
       </c>
       <c r="B119" s="2">
         <v>2</v>
@@ -3394,15 +3471,15 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>526</v>
+        <v>371</v>
       </c>
       <c r="B120" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>533</v>
+        <v>554</v>
       </c>
       <c r="B121" s="2">
         <v>1</v>
@@ -3410,7 +3487,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>466</v>
+        <v>643</v>
       </c>
       <c r="B122" s="2">
         <v>1</v>
@@ -3418,15 +3495,15 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>380</v>
+        <v>528</v>
       </c>
       <c r="B123" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>534</v>
+        <v>632</v>
       </c>
       <c r="B124" s="2">
         <v>1</v>
@@ -3434,31 +3511,31 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>501</v>
+        <v>395</v>
       </c>
       <c r="B125" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>582</v>
+        <v>374</v>
       </c>
       <c r="B126" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>474</v>
+        <v>518</v>
       </c>
       <c r="B127" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>553</v>
+        <v>416</v>
       </c>
       <c r="B128" s="2">
         <v>1</v>
@@ -3466,7 +3543,7 @@
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>540</v>
+        <v>465</v>
       </c>
       <c r="B129" s="2">
         <v>1</v>
@@ -3474,15 +3551,15 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>524</v>
+        <v>385</v>
       </c>
       <c r="B130" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>623</v>
+        <v>427</v>
       </c>
       <c r="B131" s="2">
         <v>1</v>
@@ -3490,7 +3567,7 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>428</v>
+        <v>555</v>
       </c>
       <c r="B132" s="2">
         <v>1</v>
@@ -3498,23 +3575,23 @@
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>382</v>
+        <v>559</v>
       </c>
       <c r="B133" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>610</v>
+        <v>435</v>
       </c>
       <c r="B134" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>505</v>
+        <v>656</v>
       </c>
       <c r="B135" s="2">
         <v>1</v>
@@ -3522,39 +3599,39 @@
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>448</v>
+        <v>551</v>
       </c>
       <c r="B136" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>425</v>
+        <v>441</v>
       </c>
       <c r="B137" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>408</v>
+        <v>375</v>
       </c>
       <c r="B138" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>444</v>
+        <v>494</v>
       </c>
       <c r="B139" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>506</v>
+        <v>594</v>
       </c>
       <c r="B140" s="2">
         <v>1</v>
@@ -3562,15 +3639,15 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>527</v>
+        <v>397</v>
       </c>
       <c r="B141" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>478</v>
+        <v>60</v>
       </c>
       <c r="B142" s="2">
         <v>1</v>
@@ -3578,7 +3655,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>383</v>
+        <v>519</v>
       </c>
       <c r="B143" s="2">
         <v>1</v>
@@ -3586,7 +3663,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>550</v>
+        <v>564</v>
       </c>
       <c r="B144" s="2">
         <v>1</v>
@@ -3594,15 +3671,15 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>548</v>
+        <v>657</v>
       </c>
       <c r="B145" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>591</v>
+        <v>482</v>
       </c>
       <c r="B146" s="2">
         <v>1</v>
@@ -3610,15 +3687,15 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>392</v>
+        <v>604</v>
       </c>
       <c r="B147" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>575</v>
+        <v>650</v>
       </c>
       <c r="B148" s="2">
         <v>1</v>
@@ -3626,7 +3703,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>570</v>
+        <v>456</v>
       </c>
       <c r="B149" s="2">
         <v>1</v>
@@ -3634,7 +3711,7 @@
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>547</v>
+        <v>488</v>
       </c>
       <c r="B150" s="2">
         <v>1</v>
@@ -3642,15 +3719,15 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>457</v>
+        <v>641</v>
       </c>
       <c r="B151" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>630</v>
+        <v>659</v>
       </c>
       <c r="B152" s="2">
         <v>1</v>
@@ -3658,31 +3735,31 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>393</v>
+        <v>673</v>
       </c>
       <c r="B153" s="2">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>556</v>
+        <v>662</v>
       </c>
       <c r="B154" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>440</v>
+        <v>463</v>
       </c>
       <c r="B155" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>206</v>
+        <v>663</v>
       </c>
       <c r="B156" s="2">
         <v>1</v>
@@ -3690,39 +3767,39 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>502</v>
+        <v>470</v>
       </c>
       <c r="B157" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>562</v>
+        <v>469</v>
       </c>
       <c r="B158" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>563</v>
+        <v>667</v>
       </c>
       <c r="B159" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>567</v>
+        <v>668</v>
       </c>
       <c r="B160" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>573</v>
+        <v>473</v>
       </c>
       <c r="B161" s="2">
         <v>1</v>
@@ -3730,15 +3807,15 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>433</v>
+        <v>520</v>
       </c>
       <c r="B162" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>576</v>
+        <v>640</v>
       </c>
       <c r="B163" s="2">
         <v>1</v>
@@ -3746,7 +3823,7 @@
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>577</v>
+        <v>401</v>
       </c>
       <c r="B164" s="2">
         <v>1</v>
@@ -3754,7 +3831,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>522</v>
+        <v>655</v>
       </c>
       <c r="B165" s="2">
         <v>1</v>
@@ -3762,23 +3839,23 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>529</v>
+        <v>376</v>
       </c>
       <c r="B166" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>454</v>
+        <v>660</v>
       </c>
       <c r="B167" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>581</v>
+        <v>477</v>
       </c>
       <c r="B168" s="2">
         <v>1</v>
@@ -3786,7 +3863,7 @@
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>583</v>
+        <v>479</v>
       </c>
       <c r="B169" s="2">
         <v>1</v>
@@ -3794,15 +3871,15 @@
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B170" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>638</v>
+        <v>460</v>
       </c>
       <c r="B171" s="2">
         <v>1</v>
@@ -3810,7 +3887,7 @@
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>467</v>
+        <v>578</v>
       </c>
       <c r="B172" s="2">
         <v>1</v>
@@ -3818,23 +3895,23 @@
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>468</v>
+        <v>98</v>
       </c>
       <c r="B173" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>537</v>
+        <v>99</v>
       </c>
       <c r="B174" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
       <c r="B175" s="2">
         <v>1</v>
@@ -3842,7 +3919,7 @@
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>652</v>
+        <v>565</v>
       </c>
       <c r="B176" s="2">
         <v>1</v>
@@ -3850,15 +3927,15 @@
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>450</v>
+        <v>546</v>
       </c>
       <c r="B177" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>451</v>
+        <v>489</v>
       </c>
       <c r="B178" s="2">
         <v>1</v>
@@ -3866,47 +3943,47 @@
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>483</v>
+        <v>609</v>
       </c>
       <c r="B179" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>602</v>
+        <v>491</v>
       </c>
       <c r="B180" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>453</v>
+        <v>377</v>
       </c>
       <c r="B181" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>410</v>
+        <v>497</v>
       </c>
       <c r="B182" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>495</v>
+        <v>625</v>
       </c>
       <c r="B183" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>629</v>
+        <v>492</v>
       </c>
       <c r="B184" s="2">
         <v>1</v>
@@ -3914,7 +3991,7 @@
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>569</v>
+        <v>661</v>
       </c>
       <c r="B185" s="2">
         <v>1</v>
@@ -3922,15 +3999,15 @@
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>381</v>
+        <v>512</v>
       </c>
       <c r="B186" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>411</v>
+        <v>579</v>
       </c>
       <c r="B187" s="2">
         <v>1</v>
@@ -3938,7 +4015,7 @@
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>590</v>
+        <v>644</v>
       </c>
       <c r="B188" s="2">
         <v>1</v>
@@ -3946,7 +4023,7 @@
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>571</v>
+        <v>646</v>
       </c>
       <c r="B189" s="2">
         <v>1</v>
@@ -3954,7 +4031,7 @@
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>572</v>
+        <v>516</v>
       </c>
       <c r="B190" s="2">
         <v>1</v>
@@ -3962,31 +4039,31 @@
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>541</v>
+        <v>612</v>
       </c>
       <c r="B191" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="B192" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>598</v>
+        <v>434</v>
       </c>
       <c r="B193" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>530</v>
+        <v>544</v>
       </c>
       <c r="B194" s="2">
         <v>1</v>
@@ -3994,15 +4071,15 @@
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>449</v>
+        <v>423</v>
       </c>
       <c r="B195" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>600</v>
+        <v>533</v>
       </c>
       <c r="B196" s="2">
         <v>1</v>
@@ -4010,15 +4087,15 @@
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B197" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>664</v>
+        <v>534</v>
       </c>
       <c r="B198" s="2">
         <v>1</v>
@@ -4026,15 +4103,15 @@
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>596</v>
+        <v>553</v>
       </c>
       <c r="B199" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>603</v>
+        <v>540</v>
       </c>
       <c r="B200" s="2">
         <v>1</v>
@@ -4042,39 +4119,39 @@
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>607</v>
+        <v>623</v>
       </c>
       <c r="B201" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>390</v>
+        <v>428</v>
       </c>
       <c r="B202" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>597</v>
+        <v>505</v>
       </c>
       <c r="B203" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>521</v>
+        <v>506</v>
       </c>
       <c r="B204" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>574</v>
+        <v>478</v>
       </c>
       <c r="B205" s="2">
         <v>1</v>
@@ -4082,7 +4159,7 @@
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>513</v>
+        <v>383</v>
       </c>
       <c r="B206" s="2">
         <v>1</v>
@@ -4090,15 +4167,15 @@
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>394</v>
+        <v>550</v>
       </c>
       <c r="B207" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="B208" s="2">
         <v>1</v>
@@ -4106,7 +4183,7 @@
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>480</v>
+        <v>575</v>
       </c>
       <c r="B209" s="2">
         <v>1</v>
@@ -4114,7 +4191,7 @@
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>605</v>
+        <v>570</v>
       </c>
       <c r="B210" s="2">
         <v>1</v>
@@ -4122,15 +4199,15 @@
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>592</v>
+        <v>547</v>
       </c>
       <c r="B211" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>484</v>
+        <v>630</v>
       </c>
       <c r="B212" s="2">
         <v>1</v>
@@ -4138,7 +4215,7 @@
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>599</v>
+        <v>206</v>
       </c>
       <c r="B213" s="2">
         <v>1</v>
@@ -4146,7 +4223,7 @@
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>637</v>
+        <v>573</v>
       </c>
       <c r="B214" s="2">
         <v>1</v>
@@ -4154,7 +4231,7 @@
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>633</v>
+        <v>576</v>
       </c>
       <c r="B215" s="2">
         <v>1</v>
@@ -4162,23 +4239,23 @@
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>523</v>
+        <v>577</v>
       </c>
       <c r="B216" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>421</v>
+        <v>522</v>
       </c>
       <c r="B217" s="2">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>613</v>
+        <v>581</v>
       </c>
       <c r="B218" s="2">
         <v>1</v>
@@ -4186,7 +4263,7 @@
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>614</v>
+        <v>583</v>
       </c>
       <c r="B219" s="2">
         <v>1</v>
@@ -4194,15 +4271,15 @@
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>412</v>
+        <v>638</v>
       </c>
       <c r="B220" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>645</v>
+        <v>467</v>
       </c>
       <c r="B221" s="2">
         <v>1</v>
@@ -4210,7 +4287,7 @@
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>409</v>
+        <v>627</v>
       </c>
       <c r="B222" s="2">
         <v>1</v>
@@ -4218,7 +4295,7 @@
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>485</v>
+        <v>652</v>
       </c>
       <c r="B223" s="2">
         <v>1</v>
@@ -4226,7 +4303,7 @@
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>634</v>
+        <v>451</v>
       </c>
       <c r="B224" s="2">
         <v>1</v>
@@ -4234,15 +4311,15 @@
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>406</v>
+        <v>629</v>
       </c>
       <c r="B225" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>615</v>
+        <v>569</v>
       </c>
       <c r="B226" s="2">
         <v>1</v>
@@ -4250,7 +4327,7 @@
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>608</v>
+        <v>411</v>
       </c>
       <c r="B227" s="2">
         <v>1</v>
@@ -4258,23 +4335,23 @@
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>617</v>
+        <v>590</v>
       </c>
       <c r="B228" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>429</v>
+        <v>571</v>
       </c>
       <c r="B229" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>595</v>
+        <v>572</v>
       </c>
       <c r="B230" s="2">
         <v>1</v>
@@ -4282,23 +4359,23 @@
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>621</v>
+        <v>530</v>
       </c>
       <c r="B231" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>626</v>
+        <v>600</v>
       </c>
       <c r="B232" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>628</v>
+        <v>664</v>
       </c>
       <c r="B233" s="2">
         <v>1</v>
@@ -4306,23 +4383,23 @@
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>631</v>
+        <v>603</v>
       </c>
       <c r="B234" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" t="s">
-        <v>387</v>
+        <v>574</v>
       </c>
       <c r="B235" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>558</v>
+        <v>513</v>
       </c>
       <c r="B236" s="2">
         <v>1</v>
@@ -4330,7 +4407,7 @@
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="B237" s="2">
         <v>1</v>
@@ -4338,7 +4415,7 @@
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>618</v>
+        <v>480</v>
       </c>
       <c r="B238" s="2">
         <v>1</v>
@@ -4346,7 +4423,7 @@
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>622</v>
+        <v>605</v>
       </c>
       <c r="B239" s="2">
         <v>1</v>
@@ -4354,7 +4431,7 @@
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="B240" s="2">
         <v>1</v>
@@ -4362,15 +4439,15 @@
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>552</v>
+        <v>599</v>
       </c>
       <c r="B241" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B242" s="2">
         <v>1</v>
@@ -4378,7 +4455,7 @@
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>535</v>
+        <v>633</v>
       </c>
       <c r="B243" s="2">
         <v>1</v>
@@ -4386,15 +4463,15 @@
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>587</v>
+        <v>613</v>
       </c>
       <c r="B244" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>568</v>
+        <v>614</v>
       </c>
       <c r="B245" s="2">
         <v>1</v>
@@ -4402,15 +4479,15 @@
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>422</v>
+        <v>645</v>
       </c>
       <c r="B246" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>471</v>
+        <v>409</v>
       </c>
       <c r="B247" s="2">
         <v>1</v>
@@ -4418,7 +4495,7 @@
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>531</v>
+        <v>485</v>
       </c>
       <c r="B248" s="2">
         <v>1</v>
@@ -4426,31 +4503,31 @@
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="B249" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>413</v>
+        <v>615</v>
       </c>
       <c r="B250" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B251" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>437</v>
+        <v>595</v>
       </c>
       <c r="B252" s="2">
         <v>1</v>
@@ -4458,7 +4535,7 @@
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>669</v>
+        <v>628</v>
       </c>
       <c r="B253" s="2">
         <v>1</v>
@@ -4466,15 +4543,15 @@
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B254" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>651</v>
+        <v>584</v>
       </c>
       <c r="B255" s="2">
         <v>1</v>
@@ -4482,7 +4559,7 @@
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B256" s="2">
         <v>1</v>
@@ -4490,7 +4567,7 @@
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>653</v>
+        <v>622</v>
       </c>
       <c r="B257" s="2">
         <v>1</v>
@@ -4498,23 +4575,23 @@
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>654</v>
+        <v>472</v>
       </c>
       <c r="B258" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>486</v>
+        <v>635</v>
       </c>
       <c r="B259" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>436</v>
+        <v>535</v>
       </c>
       <c r="B260" s="2">
         <v>1</v>
@@ -4522,15 +4599,15 @@
     </row>
     <row r="261" spans="1:2">
       <c r="A261" t="s">
-        <v>642</v>
+        <v>568</v>
       </c>
       <c r="B261" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" t="s">
-        <v>396</v>
+        <v>471</v>
       </c>
       <c r="B262" s="2">
         <v>1</v>
@@ -4538,7 +4615,7 @@
     </row>
     <row r="263" spans="1:2">
       <c r="A263" t="s">
-        <v>580</v>
+        <v>531</v>
       </c>
       <c r="B263" s="2">
         <v>1</v>
@@ -4546,7 +4623,7 @@
     </row>
     <row r="264" spans="1:2">
       <c r="A264" t="s">
-        <v>557</v>
+        <v>437</v>
       </c>
       <c r="B264" s="2">
         <v>1</v>
@@ -4554,7 +4631,7 @@
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>517</v>
+        <v>669</v>
       </c>
       <c r="B265" s="2">
         <v>1</v>
@@ -4562,15 +4639,15 @@
     </row>
     <row r="266" spans="1:2">
       <c r="A266" t="s">
-        <v>499</v>
+        <v>651</v>
       </c>
       <c r="B266" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" t="s">
-        <v>507</v>
+        <v>619</v>
       </c>
       <c r="B267" s="2">
         <v>1</v>
@@ -4578,7 +4655,7 @@
     </row>
     <row r="268" spans="1:2">
       <c r="A268" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="B268" s="2">
         <v>1</v>
@@ -4586,15 +4663,15 @@
     </row>
     <row r="269" spans="1:2">
       <c r="A269" t="s">
-        <v>414</v>
+        <v>436</v>
       </c>
       <c r="B269" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" t="s">
-        <v>500</v>
+        <v>396</v>
       </c>
       <c r="B270" s="2">
         <v>1</v>
@@ -4602,23 +4679,23 @@
     </row>
     <row r="271" spans="1:2">
       <c r="A271" t="s">
-        <v>445</v>
+        <v>580</v>
       </c>
       <c r="B271" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" t="s">
-        <v>542</v>
+        <v>557</v>
       </c>
       <c r="B272" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>670</v>
+        <v>517</v>
       </c>
       <c r="B273" s="2">
         <v>1</v>
@@ -4626,7 +4703,7 @@
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
-        <v>677</v>
+        <v>507</v>
       </c>
       <c r="B274" s="2">
         <v>1</v>
@@ -4634,23 +4711,23 @@
     </row>
     <row r="275" spans="1:2">
       <c r="A275" t="s">
-        <v>415</v>
+        <v>647</v>
       </c>
       <c r="B275" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="B276" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" t="s">
-        <v>648</v>
+        <v>670</v>
       </c>
       <c r="B277" s="2">
         <v>1</v>
@@ -4658,7 +4735,7 @@
     </row>
     <row r="278" spans="1:2">
       <c r="A278" t="s">
-        <v>398</v>
+        <v>677</v>
       </c>
       <c r="B278" s="2">
         <v>1</v>
@@ -4666,7 +4743,7 @@
     </row>
     <row r="279" spans="1:2">
       <c r="A279" t="s">
-        <v>525</v>
+        <v>648</v>
       </c>
       <c r="B279" s="2">
         <v>1</v>
@@ -4674,7 +4751,7 @@
     </row>
     <row r="280" spans="1:2">
       <c r="A280" t="s">
-        <v>545</v>
+        <v>398</v>
       </c>
       <c r="B280" s="2">
         <v>1</v>
@@ -4682,7 +4759,7 @@
     </row>
     <row r="281" spans="1:2">
       <c r="A281" t="s">
-        <v>671</v>
+        <v>525</v>
       </c>
       <c r="B281" s="2">
         <v>1</v>
@@ -4690,18 +4767,18 @@
     </row>
     <row r="282" spans="1:2">
       <c r="A282" t="s">
-        <v>432</v>
+        <v>545</v>
       </c>
       <c r="B282" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" t="s">
-        <v>371</v>
+        <v>671</v>
       </c>
       <c r="B283" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -4761,8 +4838,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B355">
-    <sortCondition ref="A283"/>
+  <sortState ref="A1:B291">
+    <sortCondition descending="1" ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4772,8 +4849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45EFF756-A1BB-4E25-87AA-8F79F197D039}">
   <dimension ref="A1:A400"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="A395" sqref="A395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6781,4 +6858,418 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA576171-BDC7-4FC1-B656-CFD77DA11518}">
+  <dimension ref="A1:A45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>701</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A48">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7C1D36-F8DA-431C-B1F9-6E77B3ECF3B1}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" t="s">
+        <v>681</v>
+      </c>
+      <c r="C1" t="s">
+        <v>682</v>
+      </c>
+      <c r="D1" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>689</v>
+      </c>
+      <c r="B2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2" t="s">
+        <v>686</v>
+      </c>
+      <c r="D2" t="s">
+        <v>493</v>
+      </c>
+      <c r="E2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>688</v>
+      </c>
+      <c r="B3" t="s">
+        <v>690</v>
+      </c>
+      <c r="C3" t="s">
+        <v>691</v>
+      </c>
+      <c r="D3" t="s">
+        <v>692</v>
+      </c>
+      <c r="E3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>693</v>
+      </c>
+      <c r="B4" t="s">
+        <v>694</v>
+      </c>
+      <c r="C4" t="s">
+        <v>695</v>
+      </c>
+      <c r="D4" t="s">
+        <v>696</v>
+      </c>
+      <c r="E4" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B5" t="s">
+        <v>698</v>
+      </c>
+      <c r="C5" t="s">
+        <v>699</v>
+      </c>
+      <c r="D5" t="s">
+        <v>702</v>
+      </c>
+      <c r="E5" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>701</v>
+      </c>
+      <c r="B6" t="s">
+        <v>679</v>
+      </c>
+      <c r="C6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6" t="s">
+        <v>703</v>
+      </c>
+      <c r="E6" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>448</v>
+      </c>
+      <c r="B7" t="s">
+        <v>457</v>
+      </c>
+      <c r="C7" t="s">
+        <v>562</v>
+      </c>
+      <c r="D7" t="s">
+        <v>402</v>
+      </c>
+      <c r="E7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B8" t="s">
+        <v>421</v>
+      </c>
+      <c r="C8" t="s">
+        <v>621</v>
+      </c>
+      <c r="D8" t="s">
+        <v>486</v>
+      </c>
+      <c r="E8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>422</v>
+      </c>
+      <c r="B9" t="s">
+        <v>399</v>
+      </c>
+      <c r="C9" t="s">
+        <v>381</v>
+      </c>
+      <c r="D9" t="s">
+        <v>379</v>
+      </c>
+      <c r="E9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="I1:I53">
+    <sortCondition ref="I1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>